<commit_message>
NCBI/UniProt updates + 3 curated genes
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/package__geneOncoX/geneOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{435255AE-183E-0545-AE11-E21EA2F0022F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F43D75D-4A25-DF4B-85DB-3381C0D0772B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4520" yWindow="2120" windowWidth="26840" windowHeight="15940" activeTab="4" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
+    <workbookView xWindow="4520" yWindow="2120" windowWidth="26840" windowHeight="15940" activeTab="3" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
   <sheets>
     <sheet name="panels" sheetId="1" r:id="rId1"/>
@@ -355,9 +355,6 @@
     <t>v48 (September 2022)</t>
   </si>
   <si>
-    <t>2022_03</t>
-  </si>
-  <si>
     <t>Predicted cancer driver genes / likely false positive driver genes</t>
   </si>
   <si>
@@ -371,6 +368,9 @@
   </si>
   <si>
     <t>foundation_one</t>
+  </si>
+  <si>
+    <t>2022_04</t>
   </si>
 </sst>
 </file>
@@ -973,7 +973,7 @@
         <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>38</v>
@@ -1004,16 +1004,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" t="s">
         <v>110</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="F9" t="s">
         <v>112</v>
-      </c>
-      <c r="F9" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1142,8 +1142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932642DA-7C44-1E43-949C-73113CAEBEC0}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1152,7 +1152,7 @@
     <col min="2" max="2" width="83.33203125" customWidth="1"/>
     <col min="3" max="3" width="68" customWidth="1"/>
     <col min="4" max="4" width="50.6640625" customWidth="1"/>
-    <col min="5" max="5" width="17.83203125" customWidth="1"/>
+    <col min="5" max="5" width="17.83203125" style="5" customWidth="1"/>
     <col min="6" max="7" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1169,7 +1169,7 @@
       <c r="D1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -1189,7 +1189,7 @@
       <c r="D2" t="s">
         <v>56</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="5" t="s">
         <v>6</v>
       </c>
       <c r="F2" t="s">
@@ -1209,7 +1209,7 @@
       <c r="D3" t="s">
         <v>53</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F3" t="s">
@@ -1274,6 +1274,9 @@
       <c r="B7" t="s">
         <v>79</v>
       </c>
+      <c r="E7" s="5">
+        <v>20221128</v>
+      </c>
       <c r="F7" t="s">
         <v>71</v>
       </c>
@@ -1291,7 +1294,7 @@
       <c r="D8" t="s">
         <v>75</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="5" t="s">
         <v>76</v>
       </c>
       <c r="F8" t="s">
@@ -1307,8 +1310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{032AA6E1-7CD1-0142-A783-7CD36AF8CD61}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1395,7 +1398,7 @@
         <v>101</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="F4" t="s">
         <v>99</v>

</xml_diff>

<commit_message>
UniProt + CGC update
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/package__geneOncoX/geneOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F43D75D-4A25-DF4B-85DB-3381C0D0772B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D173C4E-9A7F-1E45-B4FA-71D0D44CA4C6}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4520" yWindow="2120" windowWidth="26840" windowHeight="15940" activeTab="3" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
@@ -73,9 +73,6 @@
     <t>Cancer Gene Census</t>
   </si>
   <si>
-    <t>v96</t>
-  </si>
-  <si>
     <t>v7.0</t>
   </si>
   <si>
@@ -371,6 +368,9 @@
   </si>
   <si>
     <t>2022_04</t>
+  </si>
+  <si>
+    <t>v97</t>
   </si>
 </sst>
 </file>
@@ -794,13 +794,13 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>5</v>
@@ -814,13 +814,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
@@ -838,8 +838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35CAA087-5CE9-5744-85B8-F0D7703C76D2}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -856,13 +856,13 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>5</v>
@@ -876,16 +876,16 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
@@ -896,16 +896,16 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
@@ -913,22 +913,22 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
         <v>25</v>
       </c>
-      <c r="B4" t="s">
-        <v>26</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -936,16 +936,16 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>113</v>
       </c>
       <c r="F5" t="s">
         <v>11</v>
@@ -953,122 +953,122 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
         <v>39</v>
       </c>
-      <c r="C6" t="s">
-        <v>40</v>
-      </c>
       <c r="D6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B9" t="s">
         <v>109</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="F9" t="s">
         <v>111</v>
-      </c>
-      <c r="F9" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D10" s="2"/>
       <c r="F10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" t="s">
         <v>32</v>
       </c>
-      <c r="B11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="D11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E11" t="s">
-        <v>34</v>
-      </c>
       <c r="F11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" t="s">
         <v>89</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>90</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1101,13 +1101,13 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>5</v>
@@ -1118,19 +1118,19 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
         <v>39</v>
       </c>
-      <c r="C2" t="s">
-        <v>40</v>
-      </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1142,8 +1142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932642DA-7C44-1E43-949C-73113CAEBEC0}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1161,13 +1161,13 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>5</v>
@@ -1181,19 +1181,19 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1201,16 +1201,16 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>14</v>
+        <v>113</v>
       </c>
       <c r="F3" t="s">
         <v>11</v>
@@ -1218,87 +1218,87 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
         <v>39</v>
       </c>
-      <c r="C4" t="s">
-        <v>40</v>
-      </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" t="s">
         <v>60</v>
       </c>
-      <c r="B5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D5" t="s">
-        <v>61</v>
-      </c>
       <c r="F5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" t="s">
         <v>63</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>65</v>
-      </c>
-      <c r="F6" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E7" s="5">
         <v>20221128</v>
       </c>
       <c r="F7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" t="s">
-        <v>73</v>
-      </c>
       <c r="C8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="F8" t="s">
         <v>76</v>
-      </c>
-      <c r="F8" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1329,13 +1329,13 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>5</v>
@@ -1346,79 +1346,79 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E2" s="5">
         <v>42</v>
       </c>
       <c r="F2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" t="s">
         <v>86</v>
       </c>
-      <c r="B3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C3" t="s">
-        <v>87</v>
-      </c>
       <c r="D3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E3" s="5">
         <v>108</v>
       </c>
       <c r="F3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" t="s">
         <v>102</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>103</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="F5" t="s">
         <v>104</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="F5" t="s">
-        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cancermine v49 + custom aliases
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/package__geneOncoX/geneOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D173C4E-9A7F-1E45-B4FA-71D0D44CA4C6}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE858B3F-F9B5-1D42-B41A-232EA54280F3}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4520" yWindow="2120" windowWidth="26840" windowHeight="15940" activeTab="3" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
+    <workbookView xWindow="4520" yWindow="2120" windowWidth="26840" windowHeight="15940" activeTab="4" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
   <sheets>
     <sheet name="panels" sheetId="1" r:id="rId1"/>
@@ -349,9 +349,6 @@
     <t>Rodriguez et al, Nucleic Acids Res, 2022; 34755885</t>
   </si>
   <si>
-    <t>v48 (September 2022)</t>
-  </si>
-  <si>
     <t>Predicted cancer driver genes / likely false positive driver genes</t>
   </si>
   <si>
@@ -367,10 +364,13 @@
     <t>foundation_one</t>
   </si>
   <si>
-    <t>2022_04</t>
-  </si>
-  <si>
     <t>v97</t>
+  </si>
+  <si>
+    <t>v49 (January 2023)</t>
+  </si>
+  <si>
+    <t>2022_05</t>
   </si>
 </sst>
 </file>
@@ -839,7 +839,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -885,7 +885,7 @@
         <v>50</v>
       </c>
       <c r="E2" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
@@ -945,7 +945,7 @@
         <v>52</v>
       </c>
       <c r="E5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F5" t="s">
         <v>11</v>
@@ -973,7 +973,7 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>37</v>
@@ -1004,16 +1004,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B9" t="s">
         <v>108</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="F9" t="s">
         <v>110</v>
-      </c>
-      <c r="F9" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1142,7 +1142,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932642DA-7C44-1E43-949C-73113CAEBEC0}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -1210,7 +1210,7 @@
         <v>52</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F3" t="s">
         <v>11</v>
@@ -1310,7 +1310,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{032AA6E1-7CD1-0142-A783-7CD36AF8CD61}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -1398,7 +1398,7 @@
         <v>100</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F4" t="s">
         <v>98</v>

</xml_diff>

<commit_message>
prep march 2023 update
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/package__geneOncoX/geneOncoX/data-raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/package__geneOncoX/dev/geneOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{297A0E2F-3167-3E4B-836E-6C076BB2BA95}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2160EF9B-BCC8-DF48-9A33-869FBB6C8162}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4520" yWindow="2120" windowWidth="26840" windowHeight="15940" activeTab="4" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
+    <workbookView xWindow="4520" yWindow="2120" windowWidth="26840" windowHeight="15940" activeTab="1" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
   <sheets>
     <sheet name="panels" sheetId="1" r:id="rId1"/>
@@ -367,10 +367,10 @@
     <t>v97</t>
   </si>
   <si>
-    <t>v49 (January 2023)</t>
-  </si>
-  <si>
     <t>2022_05</t>
+  </si>
+  <si>
+    <t>v50 (March 2023)</t>
   </si>
 </sst>
 </file>
@@ -838,7 +838,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35CAA087-5CE9-5744-85B8-F0D7703C76D2}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -885,7 +885,7 @@
         <v>50</v>
       </c>
       <c r="E2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
@@ -1310,7 +1310,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{032AA6E1-7CD1-0142-A783-7CD36AF8CD61}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -1398,7 +1398,7 @@
         <v>100</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F4" t="s">
         <v>98</v>

</xml_diff>

<commit_message>
updated CGC, NCG, dbNSFP, UniProt
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/package__geneOncoX/dev/geneOncoX/data-raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/package__geneOncoX/geneOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2160EF9B-BCC8-DF48-9A33-869FBB6C8162}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3E12620-34F0-9A40-91A2-16A16C02A6EB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4520" yWindow="2120" windowWidth="26840" windowHeight="15940" activeTab="1" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
+    <workbookView xWindow="4520" yWindow="2100" windowWidth="26840" windowHeight="15940" activeTab="4" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
   <sheets>
     <sheet name="panels" sheetId="1" r:id="rId1"/>
@@ -73,9 +73,6 @@
     <t>Cancer Gene Census</t>
   </si>
   <si>
-    <t>v7.0</t>
-  </si>
-  <si>
     <t>NCBI</t>
   </si>
   <si>
@@ -307,9 +304,6 @@
     <t>Liu et al., Genome Med, 2020; 33261662</t>
   </si>
   <si>
-    <t>v4.2</t>
-  </si>
-  <si>
     <t>dbnsfp</t>
   </si>
   <si>
@@ -364,13 +358,19 @@
     <t>foundation_one</t>
   </si>
   <si>
-    <t>v97</t>
-  </si>
-  <si>
-    <t>2022_05</t>
-  </si>
-  <si>
     <t>v50 (March 2023)</t>
+  </si>
+  <si>
+    <t>v98</t>
+  </si>
+  <si>
+    <t>v4.4</t>
+  </si>
+  <si>
+    <t>v7.1</t>
+  </si>
+  <si>
+    <t>2023_02</t>
   </si>
 </sst>
 </file>
@@ -794,13 +794,13 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>5</v>
@@ -814,13 +814,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
@@ -838,8 +838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35CAA087-5CE9-5744-85B8-F0D7703C76D2}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -856,13 +856,13 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>5</v>
@@ -876,16 +876,16 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
@@ -896,16 +896,16 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>112</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
@@ -913,22 +913,22 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
         <v>24</v>
       </c>
-      <c r="B4" t="s">
-        <v>25</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -936,16 +936,16 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F5" t="s">
         <v>11</v>
@@ -953,122 +953,122 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" t="s">
         <v>38</v>
       </c>
-      <c r="C6" t="s">
-        <v>39</v>
-      </c>
       <c r="D6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B9" t="s">
+      <c r="F9" t="s">
         <v>108</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="F9" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D10" s="2"/>
       <c r="F10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" t="s">
         <v>31</v>
       </c>
-      <c r="B11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="D11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" t="s">
-        <v>33</v>
-      </c>
       <c r="F11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" t="s">
         <v>88</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>89</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1101,13 +1101,13 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>5</v>
@@ -1118,19 +1118,19 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
         <v>38</v>
       </c>
-      <c r="C2" t="s">
-        <v>39</v>
-      </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1161,13 +1161,13 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>5</v>
@@ -1181,19 +1181,19 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1201,16 +1201,16 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F3" t="s">
         <v>11</v>
@@ -1218,87 +1218,87 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s">
         <v>38</v>
       </c>
-      <c r="C4" t="s">
-        <v>39</v>
-      </c>
       <c r="D4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" t="s">
         <v>59</v>
       </c>
-      <c r="B5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" t="s">
-        <v>60</v>
-      </c>
       <c r="F5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" t="s">
         <v>62</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>64</v>
-      </c>
-      <c r="F6" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E7" s="5">
         <v>20221128</v>
       </c>
       <c r="F7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" t="s">
         <v>71</v>
       </c>
-      <c r="B8" t="s">
-        <v>72</v>
-      </c>
       <c r="C8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="F8" t="s">
         <v>75</v>
-      </c>
-      <c r="F8" t="s">
-        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1310,8 +1310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{032AA6E1-7CD1-0142-A783-7CD36AF8CD61}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1329,13 +1329,13 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>5</v>
@@ -1346,79 +1346,79 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E2" s="5">
         <v>43</v>
       </c>
       <c r="F2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" t="s">
         <v>85</v>
       </c>
-      <c r="B3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C3" t="s">
-        <v>86</v>
-      </c>
       <c r="D3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E3" s="5">
         <v>109</v>
       </c>
       <c r="F3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" t="s">
         <v>101</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="F5" t="s">
         <v>102</v>
-      </c>
-      <c r="C5" t="s">
-        <v>103</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="F5" t="s">
-        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update IntOGen, fix URL hyphens, add licensing notes
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/package__geneOncoX/geneOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3E12620-34F0-9A40-91A2-16A16C02A6EB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEBF7BC1-8D2A-A54D-95F4-96A665596D73}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4520" yWindow="2100" windowWidth="26840" windowHeight="15940" activeTab="4" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
+    <workbookView xWindow="4520" yWindow="2100" windowWidth="26840" windowHeight="15940" activeTab="1" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
   <sheets>
     <sheet name="panels" sheetId="1" r:id="rId1"/>
@@ -118,9 +118,6 @@
     <t>intogen</t>
   </si>
   <si>
-    <t>2020.02.01</t>
-  </si>
-  <si>
     <t>DNA repair gene database</t>
   </si>
   <si>
@@ -371,6 +368,9 @@
   </si>
   <si>
     <t>2023_02</t>
+  </si>
+  <si>
+    <t>2023.05.31</t>
   </si>
 </sst>
 </file>
@@ -800,7 +800,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>5</v>
@@ -814,13 +814,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
@@ -838,8 +838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35CAA087-5CE9-5744-85B8-F0D7703C76D2}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -862,7 +862,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>5</v>
@@ -876,16 +876,16 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
@@ -902,10 +902,10 @@
         <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
@@ -922,10 +922,10 @@
         <v>26</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>113</v>
       </c>
       <c r="F4" t="s">
         <v>28</v>
@@ -936,16 +936,16 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
         <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F5" t="s">
         <v>11</v>
@@ -956,13 +956,13 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
         <v>37</v>
       </c>
-      <c r="C6" t="s">
-        <v>38</v>
-      </c>
       <c r="D6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F6" t="s">
         <v>18</v>
@@ -973,13 +973,13 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F7" t="s">
         <v>21</v>
@@ -990,13 +990,13 @@
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F8" t="s">
         <v>22</v>
@@ -1004,16 +1004,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" t="s">
         <v>105</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="F9" t="s">
         <v>107</v>
-      </c>
-      <c r="F9" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1021,54 +1021,54 @@
         <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10" s="2"/>
       <c r="F10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" t="s">
         <v>30</v>
       </c>
-      <c r="B11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="D11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" t="s">
-        <v>32</v>
-      </c>
       <c r="F11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12" t="s">
         <v>87</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>88</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1107,7 +1107,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>5</v>
@@ -1121,13 +1121,13 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
         <v>37</v>
       </c>
-      <c r="C2" t="s">
-        <v>38</v>
-      </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F2" t="s">
         <v>18</v>
@@ -1167,7 +1167,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>5</v>
@@ -1181,19 +1181,19 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1201,16 +1201,16 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C3" t="s">
         <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F3" t="s">
         <v>11</v>
@@ -1221,13 +1221,13 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
         <v>37</v>
       </c>
-      <c r="C4" t="s">
-        <v>38</v>
-      </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F4" t="s">
         <v>18</v>
@@ -1235,70 +1235,70 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" t="s">
         <v>58</v>
       </c>
-      <c r="B5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" t="s">
-        <v>59</v>
-      </c>
       <c r="F5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" t="s">
         <v>61</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" t="s">
         <v>62</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>63</v>
-      </c>
-      <c r="F6" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E7" s="5">
         <v>20221128</v>
       </c>
       <c r="F7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" t="s">
         <v>70</v>
       </c>
-      <c r="B8" t="s">
-        <v>71</v>
-      </c>
       <c r="C8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="F8" t="s">
         <v>74</v>
-      </c>
-      <c r="F8" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1310,7 +1310,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{032AA6E1-7CD1-0142-A783-7CD36AF8CD61}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -1335,7 +1335,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>5</v>
@@ -1346,79 +1346,79 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E2" s="5">
         <v>43</v>
       </c>
       <c r="F2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" t="s">
         <v>84</v>
       </c>
-      <c r="B3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C3" t="s">
-        <v>85</v>
-      </c>
       <c r="D3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E3" s="5">
         <v>109</v>
       </c>
       <c r="F3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" t="s">
         <v>99</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>100</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="F5" t="s">
         <v>101</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="F5" t="s">
-        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>